<commit_message>
Small fix to volume arithmetic test
</commit_message>
<xml_diff>
--- a/cephia/cephia/test_helper/test_files/test_case_006/transfer_in.xlsx
+++ b/cephia/cephia/test_helper/test_files/test_case_006/transfer_in.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33240" yWindow="460" windowWidth="32480" windowHeight="19620" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
   <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="3">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>

</xml_diff>